<commit_message>
decide to remove nonstandard dealer offer
</commit_message>
<xml_diff>
--- a/mode/NewEngineLevelExtreme_5-50/NewEngineFormulas.xlsx
+++ b/mode/NewEngineLevelExtreme_5-50/NewEngineFormulas.xlsx
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,11 +930,11 @@
         <v>50</v>
       </c>
       <c r="F2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -948,11 +948,11 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="5">
         <f>MIN(F20:F164)</f>
-        <v>590</v>
+        <v>155</v>
       </c>
       <c r="D4" s="5">
         <f>MAX(F20:F164)</f>
-        <v>81600</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="D9" s="12">
         <v>2</v>
@@ -1028,7 +1028,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="5">
-        <v>330</v>
+        <v>370</v>
       </c>
       <c r="D10" s="12">
         <v>4</v>
@@ -1044,7 +1044,7 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="5">
-        <v>360</v>
+        <v>400</v>
       </c>
       <c r="D11" s="12">
         <v>6</v>
@@ -1060,7 +1060,7 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5">
-        <v>370</v>
+        <v>410</v>
       </c>
       <c r="D12" s="12">
         <v>8</v>
@@ -1076,7 +1076,7 @@
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5">
-        <v>380</v>
+        <v>421</v>
       </c>
       <c r="D13" s="12">
         <v>10</v>
@@ -1092,7 +1092,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="5">
-        <v>400</v>
+        <v>435</v>
       </c>
       <c r="D14" s="12">
         <v>12</v>
@@ -1108,10 +1108,10 @@
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="5">
-        <v>410</v>
+        <v>460</v>
       </c>
       <c r="D15" s="12">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E15" s="5">
         <f>IF(AND($D$6&gt;$C$14,$D$6&lt;=$C$15),1,0)*$D$15</f>
@@ -1124,14 +1124,14 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="5">
-        <v>440</v>
+        <v>600</v>
       </c>
       <c r="D16" s="12">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E16" s="5">
         <f>IF(AND($D$6&gt;$C$15,$D$6&lt;=$C$16),1,0)*$D$16</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E17" s="5">
         <f>IF(AND($D$6&gt;$C$16,$D$6&lt;=$C$17),1,0)*$D$17</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="E19" s="5">
         <f>($F$2*C19)+($H$2*D19)</f>
-        <v>870</v>
+        <v>0</v>
       </c>
       <c r="H19" s="16"/>
     </row>
@@ -1204,14 +1204,14 @@
       </c>
       <c r="F20" s="1">
         <f>($E$19+B20)*(IF(B20&lt;=$C$8,1,0)*$D$8+IF(AND(B20&gt;$C$8,B20&lt;=$C$9),1,0)*$D$9+IF(AND(B20&gt;$C$9,B20&lt;=$C$10),1,0)*$D$10+IF(AND(B20&gt;$C$10,B20&lt;=$C$11),1,0)*$D$11+IF(AND(B20&gt;$C$11,B20&lt;=$C$12),1,0)*$D$12+IF(AND(B20&gt;$C$12,B20&lt;=$C$13),1,0)*$D$13+IF(AND(B20&gt;$C$13,B20&lt;=$C$14),1,0)*$D$14+IF(AND(B20&gt;$C$14,B20&lt;=$C$15),1,0)*$D$15+IF(AND(B20&gt;$C$15,B20&lt;=$C$16),1,0)*$D$16+IF(AND(B20&gt;$C$16,B20&lt;=$C$17),1,0)*$D$17)</f>
-        <v>7380</v>
+        <v>1440</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
       </c>
       <c r="H20" s="16">
         <f>ROUND(((F20-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1223,14 +1223,14 @@
       </c>
       <c r="F21" s="1">
         <f>($E$19+B21)*(IF(B21&lt;=$C$8,1,0)*$D$8+IF(AND(B21&gt;$C$8,B21&lt;=$C$9),1,0)*$D$9+IF(AND(B21&gt;$C$9,B21&lt;=$C$10),1,0)*$D$10+IF(AND(B21&gt;$C$10,B21&lt;=$C$11),1,0)*$D$11+IF(AND(B21&gt;$C$11,B21&lt;=$C$12),1,0)*$D$12+IF(AND(B21&gt;$C$12,B21&lt;=$C$13),1,0)*$D$13+IF(AND(B21&gt;$C$13,B21&lt;=$C$14),1,0)*$D$14+IF(AND(B21&gt;$C$14,B21&lt;=$C$15),1,0)*$D$15+IF(AND(B21&gt;$C$15,B21&lt;=$C$16),1,0)*$D$16+IF(AND(B21&gt;$C$16,B21&lt;=$C$17),1,0)*$D$17)</f>
-        <v>17920</v>
+        <v>3280</v>
       </c>
       <c r="G21" s="1">
         <v>6</v>
       </c>
       <c r="H21" s="16">
         <f>ROUND(((F21-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1242,14 +1242,14 @@
       </c>
       <c r="F22" s="1">
         <f>($E$19+B22)*(IF(B22&lt;=$C$8,1,0)*$D$8+IF(AND(B22&gt;$C$8,B22&lt;=$C$9),1,0)*$D$9+IF(AND(B22&gt;$C$9,B22&lt;=$C$10),1,0)*$D$10+IF(AND(B22&gt;$C$10,B22&lt;=$C$11),1,0)*$D$11+IF(AND(B22&gt;$C$11,B22&lt;=$C$12),1,0)*$D$12+IF(AND(B22&gt;$C$12,B22&lt;=$C$13),1,0)*$D$13+IF(AND(B22&gt;$C$13,B22&lt;=$C$14),1,0)*$D$14+IF(AND(B22&gt;$C$14,B22&lt;=$C$15),1,0)*$D$15+IF(AND(B22&gt;$C$15,B22&lt;=$C$16),1,0)*$D$16+IF(AND(B22&gt;$C$16,B22&lt;=$C$17),1,0)*$D$17)</f>
-        <v>53200</v>
+        <v>9200</v>
       </c>
       <c r="G22" s="1">
         <v>10</v>
       </c>
       <c r="H22" s="16">
         <f>ROUND(((F22-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1261,14 +1261,14 @@
       </c>
       <c r="F23" s="1">
         <f>($E$19+B23)*(IF(B23&lt;=$C$8,1,0)*$D$8+IF(AND(B23&gt;$C$8,B23&lt;=$C$9),1,0)*$D$9+IF(AND(B23&gt;$C$9,B23&lt;=$C$10),1,0)*$D$10+IF(AND(B23&gt;$C$10,B23&lt;=$C$11),1,0)*$D$11+IF(AND(B23&gt;$C$11,B23&lt;=$C$12),1,0)*$D$12+IF(AND(B23&gt;$C$12,B23&lt;=$C$13),1,0)*$D$13+IF(AND(B23&gt;$C$13,B23&lt;=$C$14),1,0)*$D$14+IF(AND(B23&gt;$C$14,B23&lt;=$C$15),1,0)*$D$15+IF(AND(B23&gt;$C$15,B23&lt;=$C$16),1,0)*$D$16+IF(AND(B23&gt;$C$16,B23&lt;=$C$17),1,0)*$D$17)</f>
-        <v>55200</v>
+        <v>15300</v>
       </c>
       <c r="G23" s="1">
         <v>16</v>
       </c>
       <c r="H23" s="16">
         <f>ROUND(((F23-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
       </c>
       <c r="E24" s="5">
         <f>($F$2*C24)+($H$2*D24)</f>
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="H24" s="16"/>
     </row>
@@ -1297,14 +1297,14 @@
       </c>
       <c r="F25" s="1">
         <f>($E$24+B25)*(IF(B25&lt;=$C$8,1,0)*$D$8+IF(AND(B25&gt;$C$8,B25&lt;=$C$9),1,0)*$D$9+IF(AND(B25&gt;$C$9,B25&lt;=$C$10),1,0)*$D$10+IF(AND(B25&gt;$C$10,B25&lt;=$C$11),1,0)*$D$11+IF(AND(B25&gt;$C$11,B25&lt;=$C$12),1,0)*$D$12+IF(AND(B25&gt;$C$12,B25&lt;=$C$13),1,0)*$D$13+IF(AND(B25&gt;$C$13,B25&lt;=$C$14),1,0)*$D$14+IF(AND(B25&gt;$C$14,B25&lt;=$C$15),1,0)*$D$15+IF(AND(B25&gt;$C$15,B25&lt;=$C$16),1,0)*$D$16+IF(AND(B25&gt;$C$16,B25&lt;=$C$17),1,0)*$D$17)</f>
-        <v>10160</v>
+        <v>1480</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
       </c>
       <c r="H25" s="16">
         <f t="shared" ref="H25:H32" si="0">ROUND(((F25-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1316,14 +1316,14 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" ref="F26:F32" si="1">($E$24+B26)*(IF(B26&lt;=$C$8,1,0)*$D$8+IF(AND(B26&gt;$C$8,B26&lt;=$C$9),1,0)*$D$9+IF(AND(B26&gt;$C$9,B26&lt;=$C$10),1,0)*$D$10+IF(AND(B26&gt;$C$10,B26&lt;=$C$11),1,0)*$D$11+IF(AND(B26&gt;$C$11,B26&lt;=$C$12),1,0)*$D$12+IF(AND(B26&gt;$C$12,B26&lt;=$C$13),1,0)*$D$13+IF(AND(B26&gt;$C$13,B26&lt;=$C$14),1,0)*$D$14+IF(AND(B26&gt;$C$14,B26&lt;=$C$15),1,0)*$D$15+IF(AND(B26&gt;$C$15,B26&lt;=$C$16),1,0)*$D$16+IF(AND(B26&gt;$C$16,B26&lt;=$C$17),1,0)*$D$17)</f>
-        <v>18340</v>
+        <v>3280</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
       </c>
       <c r="H26" s="16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1335,14 +1335,14 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" si="1"/>
-        <v>21360</v>
+        <v>5220</v>
       </c>
       <c r="G27" s="1">
         <v>6</v>
       </c>
       <c r="H27" s="16">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1354,14 +1354,14 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" si="1"/>
-        <v>54000</v>
+        <v>9000</v>
       </c>
       <c r="G28" s="1">
         <v>8</v>
       </c>
       <c r="H28" s="16">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1373,14 +1373,14 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" si="1"/>
-        <v>54400</v>
+        <v>9200</v>
       </c>
       <c r="G29" s="1">
         <v>10</v>
       </c>
       <c r="H29" s="16">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1392,14 +1392,14 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" si="1"/>
-        <v>55200</v>
+        <v>14400</v>
       </c>
       <c r="G30" s="1">
         <v>14</v>
       </c>
       <c r="H30" s="16">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1411,14 +1411,14 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" si="1"/>
-        <v>56400</v>
+        <v>15300</v>
       </c>
       <c r="G31" s="1">
         <v>16</v>
       </c>
       <c r="H31" s="16">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1430,14 +1430,14 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" si="1"/>
-        <v>57200</v>
+        <v>15900</v>
       </c>
       <c r="G32" s="1">
         <v>18</v>
       </c>
       <c r="H32" s="16">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="E33" s="5">
         <f>($F$2*C33)+($H$2*D33)</f>
-        <v>870</v>
+        <v>0</v>
       </c>
       <c r="H33" s="16"/>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="F34" s="1">
         <f>($E$33+B34)*(IF(B34&lt;=$C$8,1,0)*$D$8+IF(AND(B34&gt;$C$8,B34&lt;=$C$9),1,0)*$D$9+IF(AND(B34&gt;$C$9,B34&lt;=$C$10),1,0)*$D$10+IF(AND(B34&gt;$C$10,B34&lt;=$C$11),1,0)*$D$11+IF(AND(B34&gt;$C$11,B34&lt;=$C$12),1,0)*$D$12+IF(AND(B34&gt;$C$12,B34&lt;=$C$13),1,0)*$D$13+IF(AND(B34&gt;$C$13,B34&lt;=$C$14),1,0)*$D$14+IF(AND(B34&gt;$C$14,B34&lt;=$C$15),1,0)*$D$15+IF(AND(B34&gt;$C$15,B34&lt;=$C$16),1,0)*$D$16+IF(AND(B34&gt;$C$16,B34&lt;=$C$17),1,0)*$D$17)</f>
-        <v>590</v>
+        <v>155</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
@@ -1485,14 +1485,14 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" ref="F35:F41" si="3">($E$33+B35)*(IF(B35&lt;=$C$8,1,0)*$D$8+IF(AND(B35&gt;$C$8,B35&lt;=$C$9),1,0)*$D$9+IF(AND(B35&gt;$C$9,B35&lt;=$C$10),1,0)*$D$10+IF(AND(B35&gt;$C$10,B35&lt;=$C$11),1,0)*$D$11+IF(AND(B35&gt;$C$11,B35&lt;=$C$12),1,0)*$D$12+IF(AND(B35&gt;$C$12,B35&lt;=$C$13),1,0)*$D$13+IF(AND(B35&gt;$C$13,B35&lt;=$C$14),1,0)*$D$14+IF(AND(B35&gt;$C$14,B35&lt;=$C$15),1,0)*$D$15+IF(AND(B35&gt;$C$15,B35&lt;=$C$16),1,0)*$D$16+IF(AND(B35&gt;$C$16,B35&lt;=$C$17),1,0)*$D$17)</f>
-        <v>4800</v>
+        <v>660</v>
       </c>
       <c r="G35" s="1">
         <v>6</v>
       </c>
       <c r="H35" s="16">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1504,14 +1504,14 @@
       </c>
       <c r="F36" s="1">
         <f t="shared" si="3"/>
-        <v>7380</v>
+        <v>1440</v>
       </c>
       <c r="G36" s="1">
         <v>8</v>
       </c>
       <c r="H36" s="16">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1523,14 +1523,14 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" si="3"/>
-        <v>15240</v>
+        <v>2400</v>
       </c>
       <c r="G37" s="1">
         <v>9</v>
       </c>
       <c r="H37" s="16">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1542,14 +1542,14 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" si="3"/>
-        <v>20640</v>
+        <v>4200</v>
       </c>
       <c r="G38" s="1">
         <v>10</v>
       </c>
       <c r="H38" s="16">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1561,14 +1561,14 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" si="3"/>
-        <v>53200</v>
+        <v>9200</v>
       </c>
       <c r="G39" s="1">
         <v>12</v>
       </c>
       <c r="H39" s="16">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1580,14 +1580,14 @@
       </c>
       <c r="F40" s="1">
         <f t="shared" si="3"/>
-        <v>54800</v>
+        <v>15000</v>
       </c>
       <c r="G40" s="1">
         <v>14</v>
       </c>
       <c r="H40" s="16">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1599,14 +1599,14 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" si="3"/>
-        <v>57200</v>
+        <v>16800</v>
       </c>
       <c r="G41" s="1">
         <v>16</v>
       </c>
       <c r="H41" s="16">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="E42" s="5">
         <f>($F$2*C42)+($H$2*D42)</f>
-        <v>870</v>
+        <v>0</v>
       </c>
       <c r="H42" s="16"/>
     </row>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="F43" s="1">
         <f>($E$42+B43)*(IF(B43&lt;=$C$8,1,0)*$D$8+IF(AND(B43&gt;$C$8,B43&lt;=$C$9),1,0)*$D$9+IF(AND(B43&gt;$C$9,B43&lt;=$C$10),1,0)*$D$10+IF(AND(B43&gt;$C$10,B43&lt;=$C$11),1,0)*$D$11+IF(AND(B43&gt;$C$11,B43&lt;=$C$12),1,0)*$D$12+IF(AND(B43&gt;$C$12,B43&lt;=$C$13),1,0)*$D$13+IF(AND(B43&gt;$C$13,B43&lt;=$C$14),1,0)*$D$14+IF(AND(B43&gt;$C$14,B43&lt;=$C$15),1,0)*$D$15+IF(AND(B43&gt;$C$15,B43&lt;=$C$16),1,0)*$D$16+IF(AND(B43&gt;$C$16,B43&lt;=$C$17),1,0)*$D$17)</f>
-        <v>590</v>
+        <v>155</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
@@ -1654,14 +1654,14 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" ref="F44:F49" si="5">($E$42+B44)*(IF(B44&lt;=$C$8,1,0)*$D$8+IF(AND(B44&gt;$C$8,B44&lt;=$C$9),1,0)*$D$9+IF(AND(B44&gt;$C$9,B44&lt;=$C$10),1,0)*$D$10+IF(AND(B44&gt;$C$10,B44&lt;=$C$11),1,0)*$D$11+IF(AND(B44&gt;$C$11,B44&lt;=$C$12),1,0)*$D$12+IF(AND(B44&gt;$C$12,B44&lt;=$C$13),1,0)*$D$13+IF(AND(B44&gt;$C$13,B44&lt;=$C$14),1,0)*$D$14+IF(AND(B44&gt;$C$14,B44&lt;=$C$15),1,0)*$D$15+IF(AND(B44&gt;$C$15,B44&lt;=$C$16),1,0)*$D$16+IF(AND(B44&gt;$C$16,B44&lt;=$C$17),1,0)*$D$17)</f>
-        <v>4800</v>
+        <v>660</v>
       </c>
       <c r="G44" s="1">
         <v>6</v>
       </c>
       <c r="H44" s="16">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1673,14 +1673,14 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" si="5"/>
-        <v>7380</v>
+        <v>1440</v>
       </c>
       <c r="G45" s="1">
         <v>8</v>
       </c>
       <c r="H45" s="16">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1692,14 +1692,14 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" si="5"/>
-        <v>20640</v>
+        <v>4200</v>
       </c>
       <c r="G46" s="1">
         <v>10</v>
       </c>
       <c r="H46" s="16">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1711,14 +1711,14 @@
       </c>
       <c r="F47" s="1">
         <f t="shared" si="5"/>
-        <v>52800</v>
+        <v>9000</v>
       </c>
       <c r="G47" s="1">
         <v>12</v>
       </c>
       <c r="H47" s="16">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1730,14 +1730,14 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" si="5"/>
-        <v>54800</v>
+        <v>15000</v>
       </c>
       <c r="G48" s="1">
         <v>14</v>
       </c>
       <c r="H48" s="16">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1749,14 +1749,14 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" si="5"/>
-        <v>57200</v>
+        <v>16800</v>
       </c>
       <c r="G49" s="1">
         <v>16</v>
       </c>
       <c r="H49" s="16">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="E50" s="5">
         <f>($F$2*C50)+($H$2*D50)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H50" s="16"/>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="F51" s="1">
         <f>($E$50+B51)*(IF(B51&lt;=$C$8,1,0)*$D$8+IF(AND(B51&gt;$C$8,B51&lt;=$C$9),1,0)*$D$9+IF(AND(B51&gt;$C$9,B51&lt;=$C$10),1,0)*$D$10+IF(AND(B51&gt;$C$10,B51&lt;=$C$11),1,0)*$D$11+IF(AND(B51&gt;$C$11,B51&lt;=$C$12),1,0)*$D$12+IF(AND(B51&gt;$C$12,B51&lt;=$C$13),1,0)*$D$13+IF(AND(B51&gt;$C$13,B51&lt;=$C$14),1,0)*$D$14+IF(AND(B51&gt;$C$14,B51&lt;=$C$15),1,0)*$D$15+IF(AND(B51&gt;$C$15,B51&lt;=$C$16),1,0)*$D$16+IF(AND(B51&gt;$C$16,B51&lt;=$C$17),1,0)*$D$17)</f>
-        <v>2640</v>
+        <v>640</v>
       </c>
       <c r="G51" s="1">
         <v>0</v>
@@ -1804,14 +1804,14 @@
       </c>
       <c r="F52" s="1">
         <f t="shared" ref="F52:F57" si="7">($E$50+B52)*(IF(B52&lt;=$C$8,1,0)*$D$8+IF(AND(B52&gt;$C$8,B52&lt;=$C$9),1,0)*$D$9+IF(AND(B52&gt;$C$9,B52&lt;=$C$10),1,0)*$D$10+IF(AND(B52&gt;$C$10,B52&lt;=$C$11),1,0)*$D$11+IF(AND(B52&gt;$C$11,B52&lt;=$C$12),1,0)*$D$12+IF(AND(B52&gt;$C$12,B52&lt;=$C$13),1,0)*$D$13+IF(AND(B52&gt;$C$13,B52&lt;=$C$14),1,0)*$D$14+IF(AND(B52&gt;$C$14,B52&lt;=$C$15),1,0)*$D$15+IF(AND(B52&gt;$C$15,B52&lt;=$C$16),1,0)*$D$16+IF(AND(B52&gt;$C$16,B52&lt;=$C$17),1,0)*$D$17)</f>
-        <v>8160</v>
+        <v>1440</v>
       </c>
       <c r="G52" s="1">
         <v>6</v>
       </c>
       <c r="H52" s="16">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1823,14 +1823,14 @@
       </c>
       <c r="F53" s="1">
         <f t="shared" si="7"/>
-        <v>16800</v>
+        <v>2400</v>
       </c>
       <c r="G53" s="1">
         <v>8</v>
       </c>
       <c r="H53" s="16">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1842,14 +1842,14 @@
       </c>
       <c r="F54" s="1">
         <f t="shared" si="7"/>
-        <v>23040</v>
+        <v>8800</v>
       </c>
       <c r="G54" s="1">
         <v>10</v>
       </c>
       <c r="H54" s="16">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1861,14 +1861,14 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" si="7"/>
-        <v>59200</v>
+        <v>14400</v>
       </c>
       <c r="G55" s="1">
         <v>12</v>
       </c>
       <c r="H55" s="16">
         <f t="shared" si="6"/>
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1880,14 +1880,14 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" si="7"/>
-        <v>61600</v>
+        <v>16200</v>
       </c>
       <c r="G56" s="1">
         <v>14</v>
       </c>
       <c r="H56" s="16">
         <f t="shared" si="6"/>
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1899,14 +1899,14 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" si="7"/>
-        <v>67200</v>
+        <v>27200</v>
       </c>
       <c r="G57" s="1">
         <v>16</v>
       </c>
       <c r="H57" s="16">
         <f t="shared" si="6"/>
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="E58" s="5">
         <f>($F$2*C58)+($H$2*D58)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H58" s="16"/>
     </row>
@@ -1935,14 +1935,14 @@
       </c>
       <c r="F59" s="1">
         <f>($E$58+B59)*(IF(B59&lt;=$C$8,1,0)*$D$8+IF(AND(B59&gt;$C$8,B59&lt;=$C$9),1,0)*$D$9+IF(AND(B59&gt;$C$9,B59&lt;=$C$10),1,0)*$D$10+IF(AND(B59&gt;$C$10,B59&lt;=$C$11),1,0)*$D$11+IF(AND(B59&gt;$C$11,B59&lt;=$C$12),1,0)*$D$12+IF(AND(B59&gt;$C$12,B59&lt;=$C$13),1,0)*$D$13+IF(AND(B59&gt;$C$13,B59&lt;=$C$14),1,0)*$D$14+IF(AND(B59&gt;$C$14,B59&lt;=$C$15),1,0)*$D$15+IF(AND(B59&gt;$C$15,B59&lt;=$C$16),1,0)*$D$16+IF(AND(B59&gt;$C$16,B59&lt;=$C$17),1,0)*$D$17)</f>
-        <v>8160</v>
+        <v>1440</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
       </c>
       <c r="H59" s="16">
         <f t="shared" ref="H59:H65" si="8">ROUND(((F59-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1954,14 +1954,14 @@
       </c>
       <c r="F60" s="1">
         <f t="shared" ref="F60:F65" si="9">($E$58+B60)*(IF(B60&lt;=$C$8,1,0)*$D$8+IF(AND(B60&gt;$C$8,B60&lt;=$C$9),1,0)*$D$9+IF(AND(B60&gt;$C$9,B60&lt;=$C$10),1,0)*$D$10+IF(AND(B60&gt;$C$10,B60&lt;=$C$11),1,0)*$D$11+IF(AND(B60&gt;$C$11,B60&lt;=$C$12),1,0)*$D$12+IF(AND(B60&gt;$C$12,B60&lt;=$C$13),1,0)*$D$13+IF(AND(B60&gt;$C$13,B60&lt;=$C$14),1,0)*$D$14+IF(AND(B60&gt;$C$14,B60&lt;=$C$15),1,0)*$D$15+IF(AND(B60&gt;$C$15,B60&lt;=$C$16),1,0)*$D$16+IF(AND(B60&gt;$C$16,B60&lt;=$C$17),1,0)*$D$17)</f>
-        <v>16800</v>
+        <v>2400</v>
       </c>
       <c r="G60" s="1">
         <v>6</v>
       </c>
       <c r="H60" s="16">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1973,14 +1973,14 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" si="9"/>
-        <v>23040</v>
+        <v>8800</v>
       </c>
       <c r="G61" s="1">
         <v>8</v>
       </c>
       <c r="H61" s="16">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1992,14 +1992,14 @@
       </c>
       <c r="F62" s="1">
         <f t="shared" si="9"/>
-        <v>59200</v>
+        <v>14400</v>
       </c>
       <c r="G62" s="1">
         <v>12</v>
       </c>
       <c r="H62" s="16">
         <f t="shared" si="8"/>
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2011,14 +2011,14 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" si="9"/>
-        <v>60800</v>
+        <v>15600</v>
       </c>
       <c r="G63" s="1">
         <v>16</v>
       </c>
       <c r="H63" s="16">
         <f t="shared" si="8"/>
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2030,14 +2030,14 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" si="9"/>
-        <v>62400</v>
+        <v>16800</v>
       </c>
       <c r="G64" s="1">
         <v>18</v>
       </c>
       <c r="H64" s="16">
         <f t="shared" si="8"/>
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2049,14 +2049,14 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" si="9"/>
-        <v>65600</v>
+        <v>25600</v>
       </c>
       <c r="G65" s="1">
         <v>20</v>
       </c>
       <c r="H65" s="16">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="E66" s="5">
         <f>($F$2*C66)+($H$2*D66)</f>
-        <v>918</v>
+        <v>0</v>
       </c>
       <c r="H66" s="16"/>
     </row>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="F67" s="1">
         <f>($E$66+B67)*(IF(B67&lt;=$C$8,1,0)*$D$8+IF(AND(B67&gt;$C$8,B67&lt;=$C$9),1,0)*$D$9+IF(AND(B67&gt;$C$9,B67&lt;=$C$10),1,0)*$D$10+IF(AND(B67&gt;$C$10,B67&lt;=$C$11),1,0)*$D$11+IF(AND(B67&gt;$C$11,B67&lt;=$C$12),1,0)*$D$12+IF(AND(B67&gt;$C$12,B67&lt;=$C$13),1,0)*$D$13+IF(AND(B67&gt;$C$13,B67&lt;=$C$14),1,0)*$D$14+IF(AND(B67&gt;$C$14,B67&lt;=$C$15),1,0)*$D$15+IF(AND(B67&gt;$C$15,B67&lt;=$C$16),1,0)*$D$16+IF(AND(B67&gt;$C$16,B67&lt;=$C$17),1,0)*$D$17)</f>
-        <v>2476</v>
+        <v>640</v>
       </c>
       <c r="G67" s="1">
         <v>0</v>
@@ -2104,14 +2104,14 @@
       </c>
       <c r="F68" s="1">
         <f t="shared" ref="F68:F75" si="11">($E$66+B68)*(IF(B68&lt;=$C$8,1,0)*$D$8+IF(AND(B68&gt;$C$8,B68&lt;=$C$9),1,0)*$D$9+IF(AND(B68&gt;$C$9,B68&lt;=$C$10),1,0)*$D$10+IF(AND(B68&gt;$C$10,B68&lt;=$C$11),1,0)*$D$11+IF(AND(B68&gt;$C$11,B68&lt;=$C$12),1,0)*$D$12+IF(AND(B68&gt;$C$12,B68&lt;=$C$13),1,0)*$D$13+IF(AND(B68&gt;$C$13,B68&lt;=$C$14),1,0)*$D$14+IF(AND(B68&gt;$C$14,B68&lt;=$C$15),1,0)*$D$15+IF(AND(B68&gt;$C$15,B68&lt;=$C$16),1,0)*$D$16+IF(AND(B68&gt;$C$16,B68&lt;=$C$17),1,0)*$D$17)</f>
-        <v>7668</v>
+        <v>1440</v>
       </c>
       <c r="G68" s="1">
         <v>6</v>
       </c>
       <c r="H68" s="16">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2123,14 +2123,14 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" si="11"/>
-        <v>18564</v>
+        <v>3264</v>
       </c>
       <c r="G69" s="1">
         <v>8</v>
       </c>
       <c r="H69" s="16">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2142,14 +2142,14 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" si="11"/>
-        <v>21648</v>
+        <v>5220</v>
       </c>
       <c r="G70" s="1">
         <v>10</v>
       </c>
       <c r="H70" s="16">
         <f t="shared" si="10"/>
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2161,14 +2161,14 @@
       </c>
       <c r="F71" s="1">
         <f t="shared" si="11"/>
-        <v>54960</v>
+        <v>9120</v>
       </c>
       <c r="G71" s="1">
         <v>12</v>
       </c>
       <c r="H71" s="16">
         <f t="shared" si="10"/>
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2180,14 +2180,14 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" si="11"/>
-        <v>55760</v>
+        <v>14280</v>
       </c>
       <c r="G72" s="1">
         <v>14</v>
       </c>
       <c r="H72" s="16">
         <f t="shared" si="10"/>
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2199,14 +2199,14 @@
       </c>
       <c r="F73" s="1">
         <f t="shared" si="11"/>
-        <v>57120</v>
+        <v>15300</v>
       </c>
       <c r="G73" s="1">
         <v>16</v>
       </c>
       <c r="H73" s="16">
         <f t="shared" si="10"/>
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2218,14 +2218,14 @@
       </c>
       <c r="F74" s="1">
         <f t="shared" si="11"/>
-        <v>58760</v>
+        <v>16530</v>
       </c>
       <c r="G74" s="1">
         <v>18</v>
       </c>
       <c r="H74" s="16">
         <f t="shared" si="10"/>
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2237,14 +2237,14 @@
       </c>
       <c r="F75" s="1">
         <f t="shared" si="11"/>
-        <v>60640</v>
+        <v>17940</v>
       </c>
       <c r="G75" s="1">
         <v>20</v>
       </c>
       <c r="H75" s="16">
         <f t="shared" si="10"/>
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="E76" s="5">
         <f>($F$2*C76)+($H$2*D76)</f>
-        <v>1046</v>
+        <v>0</v>
       </c>
       <c r="H76" s="16"/>
     </row>
@@ -2273,14 +2273,14 @@
       </c>
       <c r="F77" s="1">
         <f>($E$76+B77)*(IF(B77&lt;=$C$8,1,0)*$D$8+IF(AND(B77&gt;$C$8,B77&lt;=$C$9),1,0)*$D$9+IF(AND(B77&gt;$C$9,B77&lt;=$C$10),1,0)*$D$10+IF(AND(B77&gt;$C$10,B77&lt;=$C$11),1,0)*$D$11+IF(AND(B77&gt;$C$11,B77&lt;=$C$12),1,0)*$D$12+IF(AND(B77&gt;$C$12,B77&lt;=$C$13),1,0)*$D$13+IF(AND(B77&gt;$C$13,B77&lt;=$C$14),1,0)*$D$14+IF(AND(B77&gt;$C$14,B77&lt;=$C$15),1,0)*$D$15+IF(AND(B77&gt;$C$15,B77&lt;=$C$16),1,0)*$D$16+IF(AND(B77&gt;$C$16,B77&lt;=$C$17),1,0)*$D$17)</f>
-        <v>23472</v>
+        <v>4210</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
       </c>
       <c r="H77" s="16">
         <f t="shared" ref="H77:H83" si="12">ROUND(((F77-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2292,14 +2292,14 @@
       </c>
       <c r="F78" s="1">
         <f t="shared" ref="F78:F83" si="13">($E$76+B78)*(IF(B78&lt;=$C$8,1,0)*$D$8+IF(AND(B78&gt;$C$8,B78&lt;=$C$9),1,0)*$D$9+IF(AND(B78&gt;$C$9,B78&lt;=$C$10),1,0)*$D$10+IF(AND(B78&gt;$C$10,B78&lt;=$C$11),1,0)*$D$11+IF(AND(B78&gt;$C$11,B78&lt;=$C$12),1,0)*$D$12+IF(AND(B78&gt;$C$12,B78&lt;=$C$13),1,0)*$D$13+IF(AND(B78&gt;$C$13,B78&lt;=$C$14),1,0)*$D$14+IF(AND(B78&gt;$C$14,B78&lt;=$C$15),1,0)*$D$15+IF(AND(B78&gt;$C$15,B78&lt;=$C$16),1,0)*$D$16+IF(AND(B78&gt;$C$16,B78&lt;=$C$17),1,0)*$D$17)</f>
-        <v>59800</v>
+        <v>8980</v>
       </c>
       <c r="G78" s="1">
         <v>6</v>
       </c>
       <c r="H78" s="16">
         <f t="shared" si="12"/>
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2311,14 +2311,14 @@
       </c>
       <c r="F79" s="1">
         <f t="shared" si="13"/>
-        <v>60880</v>
+        <v>14280</v>
       </c>
       <c r="G79" s="1">
         <v>10</v>
       </c>
       <c r="H79" s="16">
         <f t="shared" si="12"/>
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2330,14 +2330,14 @@
       </c>
       <c r="F80" s="1">
         <f t="shared" si="13"/>
-        <v>62240</v>
+        <v>15300</v>
       </c>
       <c r="G80" s="1">
         <v>12</v>
       </c>
       <c r="H80" s="16">
         <f t="shared" si="12"/>
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2349,14 +2349,14 @@
       </c>
       <c r="F81" s="1">
         <f t="shared" si="13"/>
-        <v>62520</v>
+        <v>15510</v>
       </c>
       <c r="G81" s="1">
         <v>14</v>
       </c>
       <c r="H81" s="16">
         <f t="shared" si="12"/>
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2368,14 +2368,14 @@
       </c>
       <c r="F82" s="1">
         <f t="shared" si="13"/>
-        <v>64960</v>
+        <v>17340</v>
       </c>
       <c r="G82" s="1">
         <v>16</v>
       </c>
       <c r="H82" s="16">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="F83" s="1">
         <f t="shared" si="13"/>
-        <v>66840</v>
+        <v>25000</v>
       </c>
       <c r="G83" s="1">
         <v>20</v>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="E84" s="5">
         <f>($F$2*C84)+($H$2*D84)</f>
-        <v>960</v>
+        <v>0</v>
       </c>
       <c r="H84" s="16"/>
     </row>
@@ -2423,14 +2423,14 @@
       </c>
       <c r="F85" s="1">
         <f>($E$84+B85)*(IF(B85&lt;=$C$8,1,0)*$D$8+IF(AND(B85&gt;$C$8,B85&lt;=$C$9),1,0)*$D$9+IF(AND(B85&gt;$C$9,B85&lt;=$C$10),1,0)*$D$10+IF(AND(B85&gt;$C$10,B85&lt;=$C$11),1,0)*$D$11+IF(AND(B85&gt;$C$11,B85&lt;=$C$12),1,0)*$D$12+IF(AND(B85&gt;$C$12,B85&lt;=$C$13),1,0)*$D$13+IF(AND(B85&gt;$C$13,B85&lt;=$C$14),1,0)*$D$14+IF(AND(B85&gt;$C$14,B85&lt;=$C$15),1,0)*$D$15+IF(AND(B85&gt;$C$15,B85&lt;=$C$16),1,0)*$D$16+IF(AND(B85&gt;$C$16,B85&lt;=$C$17),1,0)*$D$17)</f>
-        <v>22400</v>
+        <v>8800</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
       </c>
       <c r="H85" s="16">
         <f>ROUND(((F85-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2442,14 +2442,14 @@
       </c>
       <c r="F86" s="1">
         <f>($E$84+B86)*(IF(B86&lt;=$C$8,1,0)*$D$8+IF(AND(B86&gt;$C$8,B86&lt;=$C$9),1,0)*$D$9+IF(AND(B86&gt;$C$9,B86&lt;=$C$10),1,0)*$D$10+IF(AND(B86&gt;$C$10,B86&lt;=$C$11),1,0)*$D$11+IF(AND(B86&gt;$C$11,B86&lt;=$C$12),1,0)*$D$12+IF(AND(B86&gt;$C$12,B86&lt;=$C$13),1,0)*$D$13+IF(AND(B86&gt;$C$13,B86&lt;=$C$14),1,0)*$D$14+IF(AND(B86&gt;$C$14,B86&lt;=$C$15),1,0)*$D$15+IF(AND(B86&gt;$C$15,B86&lt;=$C$16),1,0)*$D$16+IF(AND(B86&gt;$C$16,B86&lt;=$C$17),1,0)*$D$17)</f>
-        <v>57600</v>
+        <v>14400</v>
       </c>
       <c r="G86" s="1">
         <v>10</v>
       </c>
       <c r="H86" s="16">
         <f>ROUND(((F86-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2461,14 +2461,14 @@
       </c>
       <c r="F87" s="1">
         <f>($E$84+B87)*(IF(B87&lt;=$C$8,1,0)*$D$8+IF(AND(B87&gt;$C$8,B87&lt;=$C$9),1,0)*$D$9+IF(AND(B87&gt;$C$9,B87&lt;=$C$10),1,0)*$D$10+IF(AND(B87&gt;$C$10,B87&lt;=$C$11),1,0)*$D$11+IF(AND(B87&gt;$C$11,B87&lt;=$C$12),1,0)*$D$12+IF(AND(B87&gt;$C$12,B87&lt;=$C$13),1,0)*$D$13+IF(AND(B87&gt;$C$13,B87&lt;=$C$14),1,0)*$D$14+IF(AND(B87&gt;$C$14,B87&lt;=$C$15),1,0)*$D$15+IF(AND(B87&gt;$C$15,B87&lt;=$C$16),1,0)*$D$16+IF(AND(B87&gt;$C$16,B87&lt;=$C$17),1,0)*$D$17)</f>
-        <v>59200</v>
+        <v>15600</v>
       </c>
       <c r="G87" s="1">
         <v>16</v>
       </c>
       <c r="H87" s="16">
         <f>ROUND(((F87-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="E88" s="5">
         <f>($F$2*C88)+($H$2*D88)</f>
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="H88" s="16"/>
     </row>
@@ -2497,14 +2497,14 @@
       </c>
       <c r="F89" s="1">
         <f>($E$88+B89)*(IF(B89&lt;=$C$8,1,0)*$D$8+IF(AND(B89&gt;$C$8,B89&lt;=$C$9),1,0)*$D$9+IF(AND(B89&gt;$C$9,B89&lt;=$C$10),1,0)*$D$10+IF(AND(B89&gt;$C$10,B89&lt;=$C$11),1,0)*$D$11+IF(AND(B89&gt;$C$11,B89&lt;=$C$12),1,0)*$D$12+IF(AND(B89&gt;$C$12,B89&lt;=$C$13),1,0)*$D$13+IF(AND(B89&gt;$C$13,B89&lt;=$C$14),1,0)*$D$14+IF(AND(B89&gt;$C$14,B89&lt;=$C$15),1,0)*$D$15+IF(AND(B89&gt;$C$15,B89&lt;=$C$16),1,0)*$D$16+IF(AND(B89&gt;$C$16,B89&lt;=$C$17),1,0)*$D$17)</f>
-        <v>12200</v>
+        <v>2280</v>
       </c>
       <c r="G89" s="1">
         <v>0</v>
       </c>
       <c r="H89" s="16">
         <f>ROUND(((F89-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2516,14 +2516,14 @@
       </c>
       <c r="F90" s="1">
         <f>($E$88+B90)*(IF(B90&lt;=$C$8,1,0)*$D$8+IF(AND(B90&gt;$C$8,B90&lt;=$C$9),1,0)*$D$9+IF(AND(B90&gt;$C$9,B90&lt;=$C$10),1,0)*$D$10+IF(AND(B90&gt;$C$10,B90&lt;=$C$11),1,0)*$D$11+IF(AND(B90&gt;$C$11,B90&lt;=$C$12),1,0)*$D$12+IF(AND(B90&gt;$C$12,B90&lt;=$C$13),1,0)*$D$13+IF(AND(B90&gt;$C$13,B90&lt;=$C$14),1,0)*$D$14+IF(AND(B90&gt;$C$14,B90&lt;=$C$15),1,0)*$D$15+IF(AND(B90&gt;$C$15,B90&lt;=$C$16),1,0)*$D$16+IF(AND(B90&gt;$C$16,B90&lt;=$C$17),1,0)*$D$17)</f>
-        <v>20320</v>
+        <v>5160</v>
       </c>
       <c r="G90" s="1">
         <v>10</v>
       </c>
       <c r="H90" s="16">
         <f>ROUND(((F90-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2535,14 +2535,14 @@
       </c>
       <c r="F91" s="1">
         <f>($E$88+B91)*(IF(B91&lt;=$C$8,1,0)*$D$8+IF(AND(B91&gt;$C$8,B91&lt;=$C$9),1,0)*$D$9+IF(AND(B91&gt;$C$9,B91&lt;=$C$10),1,0)*$D$10+IF(AND(B91&gt;$C$10,B91&lt;=$C$11),1,0)*$D$11+IF(AND(B91&gt;$C$11,B91&lt;=$C$12),1,0)*$D$12+IF(AND(B91&gt;$C$12,B91&lt;=$C$13),1,0)*$D$13+IF(AND(B91&gt;$C$13,B91&lt;=$C$14),1,0)*$D$14+IF(AND(B91&gt;$C$14,B91&lt;=$C$15),1,0)*$D$15+IF(AND(B91&gt;$C$15,B91&lt;=$C$16),1,0)*$D$16+IF(AND(B91&gt;$C$16,B91&lt;=$C$17),1,0)*$D$17)</f>
-        <v>52000</v>
+        <v>9200</v>
       </c>
       <c r="G91" s="1">
         <v>16</v>
       </c>
       <c r="H91" s="16">
         <f>ROUND(((F91-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="E92" s="5">
         <f>($F$2*C92)+($H$2*D92)</f>
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="H92" s="16"/>
     </row>
@@ -2571,14 +2571,14 @@
       </c>
       <c r="F93" s="1">
         <f t="shared" ref="F93:F98" si="14">($E$92+B93)*(IF(B93&lt;=$C$8,1,0)*$D$8+IF(AND(B93&gt;$C$8,B93&lt;=$C$9),1,0)*$D$9+IF(AND(B93&gt;$C$9,B93&lt;=$C$10),1,0)*$D$10+IF(AND(B93&gt;$C$10,B93&lt;=$C$11),1,0)*$D$11+IF(AND(B93&gt;$C$11,B93&lt;=$C$12),1,0)*$D$12+IF(AND(B93&gt;$C$12,B93&lt;=$C$13),1,0)*$D$13+IF(AND(B93&gt;$C$13,B93&lt;=$C$14),1,0)*$D$14+IF(AND(B93&gt;$C$14,B93&lt;=$C$15),1,0)*$D$15+IF(AND(B93&gt;$C$15,B93&lt;=$C$16),1,0)*$D$16+IF(AND(B93&gt;$C$16,B93&lt;=$C$17),1,0)*$D$17)</f>
-        <v>12800</v>
+        <v>2280</v>
       </c>
       <c r="G93" s="1">
         <v>0</v>
       </c>
       <c r="H93" s="16">
         <f t="shared" ref="H93:H98" si="15">ROUND(((F93-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2590,14 +2590,14 @@
       </c>
       <c r="F94" s="1">
         <f t="shared" si="14"/>
-        <v>21280</v>
+        <v>5160</v>
       </c>
       <c r="G94" s="1">
         <v>10</v>
       </c>
       <c r="H94" s="16">
         <f t="shared" si="15"/>
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2609,14 +2609,14 @@
       </c>
       <c r="F95" s="1">
         <f t="shared" si="14"/>
-        <v>21440</v>
+        <v>8800</v>
       </c>
       <c r="G95" s="1">
         <v>12</v>
       </c>
       <c r="H95" s="16">
         <f t="shared" si="15"/>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2628,14 +2628,14 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" si="14"/>
-        <v>54400</v>
+        <v>9200</v>
       </c>
       <c r="G96" s="1">
         <v>14</v>
       </c>
       <c r="H96" s="16">
         <f t="shared" si="15"/>
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2647,14 +2647,14 @@
       </c>
       <c r="F97" s="1">
         <f t="shared" si="14"/>
-        <v>55200</v>
+        <v>14400</v>
       </c>
       <c r="G97" s="1">
         <v>16</v>
       </c>
       <c r="H97" s="16">
         <f t="shared" si="15"/>
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2666,14 +2666,14 @@
       </c>
       <c r="F98" s="1">
         <f t="shared" si="14"/>
-        <v>56800</v>
+        <v>15600</v>
       </c>
       <c r="G98" s="1">
         <v>18</v>
       </c>
       <c r="H98" s="16">
         <f t="shared" si="15"/>
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -2689,7 +2689,7 @@
       </c>
       <c r="E99" s="5">
         <f>($F$2*C99)+($H$2*D99)</f>
-        <v>1090</v>
+        <v>0</v>
       </c>
       <c r="H99" s="16"/>
     </row>
@@ -2702,14 +2702,14 @@
       </c>
       <c r="F100" s="1">
         <f>($E$99+B100)*(IF(B100&lt;=$C$8,1,0)*$D$8+IF(AND(B100&gt;$C$8,B100&lt;=$C$9),1,0)*$D$9+IF(AND(B100&gt;$C$9,B100&lt;=$C$10),1,0)*$D$10+IF(AND(B100&gt;$C$10,B100&lt;=$C$11),1,0)*$D$11+IF(AND(B100&gt;$C$11,B100&lt;=$C$12),1,0)*$D$12+IF(AND(B100&gt;$C$12,B100&lt;=$C$13),1,0)*$D$13+IF(AND(B100&gt;$C$13,B100&lt;=$C$14),1,0)*$D$14+IF(AND(B100&gt;$C$14,B100&lt;=$C$15),1,0)*$D$15+IF(AND(B100&gt;$C$15,B100&lt;=$C$16),1,0)*$D$16+IF(AND(B100&gt;$C$16,B100&lt;=$C$17),1,0)*$D$17)</f>
-        <v>8700</v>
+        <v>1440</v>
       </c>
       <c r="G100" s="1">
         <v>0</v>
       </c>
       <c r="H100" s="16">
         <f t="shared" ref="H100:H111" si="16">ROUND(((F100-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2721,14 +2721,14 @@
       </c>
       <c r="F101" s="1">
         <f t="shared" ref="F101:F111" si="17">($E$99+B101)*(IF(B101&lt;=$C$8,1,0)*$D$8+IF(AND(B101&gt;$C$8,B101&lt;=$C$9),1,0)*$D$9+IF(AND(B101&gt;$C$9,B101&lt;=$C$10),1,0)*$D$10+IF(AND(B101&gt;$C$10,B101&lt;=$C$11),1,0)*$D$11+IF(AND(B101&gt;$C$11,B101&lt;=$C$12),1,0)*$D$12+IF(AND(B101&gt;$C$12,B101&lt;=$C$13),1,0)*$D$13+IF(AND(B101&gt;$C$13,B101&lt;=$C$14),1,0)*$D$14+IF(AND(B101&gt;$C$14,B101&lt;=$C$15),1,0)*$D$15+IF(AND(B101&gt;$C$15,B101&lt;=$C$16),1,0)*$D$16+IF(AND(B101&gt;$C$16,B101&lt;=$C$17),1,0)*$D$17)</f>
-        <v>14700</v>
+        <v>2280</v>
       </c>
       <c r="G101" s="1">
         <v>8</v>
       </c>
       <c r="H101" s="16">
         <f t="shared" si="16"/>
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2740,14 +2740,14 @@
       </c>
       <c r="F102" s="1">
         <f t="shared" si="17"/>
-        <v>17880</v>
+        <v>2400</v>
       </c>
       <c r="G102" s="1">
         <v>8</v>
       </c>
       <c r="H102" s="16">
         <f t="shared" si="16"/>
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2759,14 +2759,14 @@
       </c>
       <c r="F103" s="1">
         <f t="shared" si="17"/>
-        <v>24160</v>
+        <v>4200</v>
       </c>
       <c r="G103" s="1">
         <v>10</v>
       </c>
       <c r="H103" s="16">
         <f t="shared" si="16"/>
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="F104" s="1">
         <f t="shared" si="17"/>
-        <v>24480</v>
+        <v>8800</v>
       </c>
       <c r="G104" s="1">
         <v>12</v>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="F105" s="1">
         <f t="shared" si="17"/>
-        <v>24480</v>
+        <v>8800</v>
       </c>
       <c r="G105" s="1">
         <v>12</v>
@@ -2816,14 +2816,14 @@
       </c>
       <c r="F106" s="1">
         <f t="shared" si="17"/>
-        <v>62800</v>
+        <v>14400</v>
       </c>
       <c r="G106" s="1">
         <v>14</v>
       </c>
       <c r="H106" s="16">
         <f t="shared" si="16"/>
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2835,14 +2835,14 @@
       </c>
       <c r="F107" s="1">
         <f t="shared" si="17"/>
-        <v>62800</v>
+        <v>14400</v>
       </c>
       <c r="G107" s="1">
         <v>14</v>
       </c>
       <c r="H107" s="16">
         <f t="shared" si="16"/>
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2854,14 +2854,14 @@
       </c>
       <c r="F108" s="1">
         <f t="shared" si="17"/>
-        <v>63600</v>
+        <v>15000</v>
       </c>
       <c r="G108" s="1">
         <v>16</v>
       </c>
       <c r="H108" s="16">
         <f t="shared" si="16"/>
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2873,14 +2873,14 @@
       </c>
       <c r="F109" s="1">
         <f t="shared" si="17"/>
-        <v>66000</v>
+        <v>16800</v>
       </c>
       <c r="G109" s="1">
         <v>18</v>
       </c>
       <c r="H109" s="16">
         <f t="shared" si="16"/>
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="110" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2892,14 +2892,14 @@
       </c>
       <c r="F110" s="1">
         <f t="shared" si="17"/>
-        <v>68400</v>
+        <v>24800</v>
       </c>
       <c r="G110" s="1">
         <v>20</v>
       </c>
       <c r="H110" s="16">
         <f t="shared" si="16"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2911,14 +2911,14 @@
       </c>
       <c r="F111" s="1">
         <f t="shared" si="17"/>
-        <v>72800</v>
+        <v>29200</v>
       </c>
       <c r="G111" s="1">
         <v>25</v>
       </c>
       <c r="H111" s="16">
         <f t="shared" si="16"/>
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="E112" s="5">
         <f>($F$2*C112)+($H$2*D112)</f>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="H112" s="16"/>
     </row>
@@ -2947,14 +2947,14 @@
       </c>
       <c r="F113" s="1">
         <f>($E$112+B113)*(IF(B113&lt;=$C$8,1,0)*$D$8+IF(AND(B113&gt;$C$8,B113&lt;=$C$9),1,0)*$D$9+IF(AND(B113&gt;$C$9,B113&lt;=$C$10),1,0)*$D$10+IF(AND(B113&gt;$C$10,B113&lt;=$C$11),1,0)*$D$11+IF(AND(B113&gt;$C$11,B113&lt;=$C$12),1,0)*$D$12+IF(AND(B113&gt;$C$12,B113&lt;=$C$13),1,0)*$D$13+IF(AND(B113&gt;$C$13,B113&lt;=$C$14),1,0)*$D$14+IF(AND(B113&gt;$C$14,B113&lt;=$C$15),1,0)*$D$15+IF(AND(B113&gt;$C$15,B113&lt;=$C$16),1,0)*$D$16+IF(AND(B113&gt;$C$16,B113&lt;=$C$17),1,0)*$D$17)</f>
-        <v>11760</v>
+        <v>1480</v>
       </c>
       <c r="G113" s="1">
         <v>0</v>
       </c>
       <c r="H113" s="16">
         <f t="shared" ref="H113:H120" si="18">ROUND(((F113-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2966,14 +2966,14 @@
       </c>
       <c r="F114" s="1">
         <f t="shared" ref="F114:F120" si="19">($E$112+B114)*(IF(B114&lt;=$C$8,1,0)*$D$8+IF(AND(B114&gt;$C$8,B114&lt;=$C$9),1,0)*$D$9+IF(AND(B114&gt;$C$9,B114&lt;=$C$10),1,0)*$D$10+IF(AND(B114&gt;$C$10,B114&lt;=$C$11),1,0)*$D$11+IF(AND(B114&gt;$C$11,B114&lt;=$C$12),1,0)*$D$12+IF(AND(B114&gt;$C$12,B114&lt;=$C$13),1,0)*$D$13+IF(AND(B114&gt;$C$13,B114&lt;=$C$14),1,0)*$D$14+IF(AND(B114&gt;$C$14,B114&lt;=$C$15),1,0)*$D$15+IF(AND(B114&gt;$C$15,B114&lt;=$C$16),1,0)*$D$16+IF(AND(B114&gt;$C$16,B114&lt;=$C$17),1,0)*$D$17)</f>
-        <v>21140</v>
+        <v>3280</v>
       </c>
       <c r="G114" s="1">
         <v>6</v>
       </c>
       <c r="H114" s="16">
         <f t="shared" si="18"/>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2985,14 +2985,14 @@
       </c>
       <c r="F115" s="1">
         <f t="shared" si="19"/>
-        <v>62000</v>
+        <v>9000</v>
       </c>
       <c r="G115" s="1">
         <v>10</v>
       </c>
       <c r="H115" s="16">
         <f t="shared" si="18"/>
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3004,14 +3004,14 @@
       </c>
       <c r="F116" s="1">
         <f t="shared" si="19"/>
-        <v>64000</v>
+        <v>15000</v>
       </c>
       <c r="G116" s="1">
         <v>12</v>
       </c>
       <c r="H116" s="16">
         <f t="shared" si="18"/>
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3023,14 +3023,14 @@
       </c>
       <c r="F117" s="1">
         <f t="shared" si="19"/>
-        <v>64800</v>
+        <v>15600</v>
       </c>
       <c r="G117" s="1">
         <v>15</v>
       </c>
       <c r="H117" s="16">
         <f t="shared" si="18"/>
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3042,14 +3042,14 @@
       </c>
       <c r="F118" s="1">
         <f t="shared" si="19"/>
-        <v>67200</v>
+        <v>17400</v>
       </c>
       <c r="G118" s="1">
         <v>18</v>
       </c>
       <c r="H118" s="16">
         <f t="shared" si="18"/>
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="F119" s="1">
         <f t="shared" si="19"/>
-        <v>70000</v>
+        <v>26000</v>
       </c>
       <c r="G119" s="1">
         <v>20</v>
@@ -3080,14 +3080,14 @@
       </c>
       <c r="F120" s="1">
         <f t="shared" si="19"/>
-        <v>73200</v>
+        <v>29200</v>
       </c>
       <c r="G120" s="1">
         <v>25</v>
       </c>
       <c r="H120" s="16">
         <f t="shared" si="18"/>
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="E121" s="5">
         <f>($F$2*C121)+($H$2*D121)</f>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="H121" s="16"/>
     </row>
@@ -3116,14 +3116,14 @@
       </c>
       <c r="F122" s="1">
         <f>($E$121+B122)*(IF(B122&lt;=$C$8,1,0)*$D$8+IF(AND(B122&gt;$C$8,B122&lt;=$C$9),1,0)*$D$9+IF(AND(B122&gt;$C$9,B122&lt;=$C$10),1,0)*$D$10+IF(AND(B122&gt;$C$10,B122&lt;=$C$11),1,0)*$D$11+IF(AND(B122&gt;$C$11,B122&lt;=$C$12),1,0)*$D$12+IF(AND(B122&gt;$C$12,B122&lt;=$C$13),1,0)*$D$13+IF(AND(B122&gt;$C$13,B122&lt;=$C$14),1,0)*$D$14+IF(AND(B122&gt;$C$14,B122&lt;=$C$15),1,0)*$D$15+IF(AND(B122&gt;$C$15,B122&lt;=$C$16),1,0)*$D$16+IF(AND(B122&gt;$C$16,B122&lt;=$C$17),1,0)*$D$17)</f>
-        <v>11760</v>
+        <v>1480</v>
       </c>
       <c r="G122" s="1">
         <v>0</v>
       </c>
       <c r="H122" s="16">
         <f t="shared" ref="H122:H129" si="20">ROUND(((F122-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3135,14 +3135,14 @@
       </c>
       <c r="F123" s="1">
         <f t="shared" ref="F123:F129" si="21">($E$121+B123)*(IF(B123&lt;=$C$8,1,0)*$D$8+IF(AND(B123&gt;$C$8,B123&lt;=$C$9),1,0)*$D$9+IF(AND(B123&gt;$C$9,B123&lt;=$C$10),1,0)*$D$10+IF(AND(B123&gt;$C$10,B123&lt;=$C$11),1,0)*$D$11+IF(AND(B123&gt;$C$11,B123&lt;=$C$12),1,0)*$D$12+IF(AND(B123&gt;$C$12,B123&lt;=$C$13),1,0)*$D$13+IF(AND(B123&gt;$C$13,B123&lt;=$C$14),1,0)*$D$14+IF(AND(B123&gt;$C$14,B123&lt;=$C$15),1,0)*$D$15+IF(AND(B123&gt;$C$15,B123&lt;=$C$16),1,0)*$D$16+IF(AND(B123&gt;$C$16,B123&lt;=$C$17),1,0)*$D$17)</f>
-        <v>21140</v>
+        <v>3280</v>
       </c>
       <c r="G123" s="1">
         <v>6</v>
       </c>
       <c r="H123" s="16">
         <f t="shared" si="20"/>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3154,14 +3154,14 @@
       </c>
       <c r="F124" s="1">
         <f t="shared" si="21"/>
-        <v>62000</v>
+        <v>9000</v>
       </c>
       <c r="G124" s="1">
         <v>10</v>
       </c>
       <c r="H124" s="16">
         <f t="shared" si="20"/>
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3173,14 +3173,14 @@
       </c>
       <c r="F125" s="1">
         <f t="shared" si="21"/>
-        <v>64000</v>
+        <v>15000</v>
       </c>
       <c r="G125" s="1">
         <v>12</v>
       </c>
       <c r="H125" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="126" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3192,14 +3192,14 @@
       </c>
       <c r="F126" s="1">
         <f t="shared" si="21"/>
-        <v>64800</v>
+        <v>15600</v>
       </c>
       <c r="G126" s="1">
         <v>15</v>
       </c>
       <c r="H126" s="16">
         <f t="shared" si="20"/>
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="127" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3211,14 +3211,14 @@
       </c>
       <c r="F127" s="1">
         <f t="shared" si="21"/>
-        <v>67200</v>
+        <v>17400</v>
       </c>
       <c r="G127" s="1">
         <v>18</v>
       </c>
       <c r="H127" s="16">
         <f t="shared" si="20"/>
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3230,7 +3230,7 @@
       </c>
       <c r="F128" s="1">
         <f t="shared" si="21"/>
-        <v>70000</v>
+        <v>26000</v>
       </c>
       <c r="G128" s="1">
         <v>20</v>
@@ -3249,14 +3249,14 @@
       </c>
       <c r="F129" s="1">
         <f t="shared" si="21"/>
-        <v>73200</v>
+        <v>29200</v>
       </c>
       <c r="G129" s="1">
         <v>25</v>
       </c>
       <c r="H129" s="16">
         <f t="shared" si="20"/>
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="E130" s="5">
         <f>($F$2*C130)+($H$2*D130)</f>
-        <v>1090</v>
+        <v>0</v>
       </c>
       <c r="H130" s="16"/>
     </row>
@@ -3285,14 +3285,14 @@
       </c>
       <c r="F131" s="1">
         <f>($E$130+B131)*(IF(B131&lt;=$C$8,1,0)*$D$8+IF(AND(B131&gt;$C$8,B131&lt;=$C$9),1,0)*$D$9+IF(AND(B131&gt;$C$9,B131&lt;=$C$10),1,0)*$D$10+IF(AND(B131&gt;$C$10,B131&lt;=$C$11),1,0)*$D$11+IF(AND(B131&gt;$C$11,B131&lt;=$C$12),1,0)*$D$12+IF(AND(B131&gt;$C$12,B131&lt;=$C$13),1,0)*$D$13+IF(AND(B131&gt;$C$13,B131&lt;=$C$14),1,0)*$D$14+IF(AND(B131&gt;$C$14,B131&lt;=$C$15),1,0)*$D$15+IF(AND(B131&gt;$C$15,B131&lt;=$C$16),1,0)*$D$16+IF(AND(B131&gt;$C$16,B131&lt;=$C$17),1,0)*$D$17)</f>
-        <v>8700</v>
+        <v>1440</v>
       </c>
       <c r="G131" s="1">
         <v>0</v>
       </c>
       <c r="H131" s="16">
         <f t="shared" ref="H131:H149" si="22">ROUND(((F131-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3304,14 +3304,14 @@
       </c>
       <c r="F132" s="1">
         <f t="shared" ref="F132:F149" si="23">($E$130+B132)*(IF(B132&lt;=$C$8,1,0)*$D$8+IF(AND(B132&gt;$C$8,B132&lt;=$C$9),1,0)*$D$9+IF(AND(B132&gt;$C$9,B132&lt;=$C$10),1,0)*$D$10+IF(AND(B132&gt;$C$10,B132&lt;=$C$11),1,0)*$D$11+IF(AND(B132&gt;$C$11,B132&lt;=$C$12),1,0)*$D$12+IF(AND(B132&gt;$C$12,B132&lt;=$C$13),1,0)*$D$13+IF(AND(B132&gt;$C$13,B132&lt;=$C$14),1,0)*$D$14+IF(AND(B132&gt;$C$14,B132&lt;=$C$15),1,0)*$D$15+IF(AND(B132&gt;$C$15,B132&lt;=$C$16),1,0)*$D$16+IF(AND(B132&gt;$C$16,B132&lt;=$C$17),1,0)*$D$17)</f>
-        <v>11680</v>
+        <v>1480</v>
       </c>
       <c r="G132" s="1">
         <v>3</v>
       </c>
       <c r="H132" s="16">
         <f t="shared" si="22"/>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="133" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3323,14 +3323,14 @@
       </c>
       <c r="F133" s="1">
         <f t="shared" si="23"/>
-        <v>14700</v>
+        <v>2280</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
       </c>
       <c r="H133" s="16">
         <f t="shared" si="22"/>
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3342,14 +3342,14 @@
       </c>
       <c r="F134" s="1">
         <f t="shared" si="23"/>
-        <v>17880</v>
+        <v>2400</v>
       </c>
       <c r="G134" s="1">
         <v>8</v>
       </c>
       <c r="H134" s="16">
         <f t="shared" si="22"/>
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3361,14 +3361,14 @@
       </c>
       <c r="F135" s="1">
         <f t="shared" si="23"/>
-        <v>21000</v>
+        <v>3280</v>
       </c>
       <c r="G135" s="1">
         <v>12</v>
       </c>
       <c r="H135" s="16">
         <f t="shared" si="22"/>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3380,14 +3380,14 @@
       </c>
       <c r="F136" s="1">
         <f t="shared" si="23"/>
-        <v>24160</v>
+        <v>4200</v>
       </c>
       <c r="G136" s="1">
         <v>10</v>
       </c>
       <c r="H136" s="16">
         <f t="shared" si="22"/>
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="F137" s="1">
         <f t="shared" si="23"/>
-        <v>24480</v>
+        <v>8800</v>
       </c>
       <c r="G137" s="1">
         <v>12</v>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="F138" s="1">
         <f t="shared" si="23"/>
-        <v>24480</v>
+        <v>8800</v>
       </c>
       <c r="G138" s="1">
         <v>12</v>
@@ -3437,14 +3437,14 @@
       </c>
       <c r="F139" s="1">
         <f t="shared" si="23"/>
-        <v>61600</v>
+        <v>9000</v>
       </c>
       <c r="G139" s="1">
         <v>14</v>
       </c>
       <c r="H139" s="16">
         <f t="shared" si="22"/>
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3456,14 +3456,14 @@
       </c>
       <c r="F140" s="1">
         <f t="shared" si="23"/>
-        <v>62800</v>
+        <v>14400</v>
       </c>
       <c r="G140" s="1">
         <v>14</v>
       </c>
       <c r="H140" s="16">
         <f t="shared" si="22"/>
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3475,14 +3475,14 @@
       </c>
       <c r="F141" s="1">
         <f t="shared" si="23"/>
-        <v>62800</v>
+        <v>14400</v>
       </c>
       <c r="G141" s="1">
         <v>14</v>
       </c>
       <c r="H141" s="16">
         <f t="shared" si="22"/>
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="142" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3494,14 +3494,14 @@
       </c>
       <c r="F142" s="1">
         <f t="shared" si="23"/>
-        <v>63200</v>
+        <v>14700</v>
       </c>
       <c r="G142" s="1">
         <v>15</v>
       </c>
       <c r="H142" s="16">
         <f t="shared" si="22"/>
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="143" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3513,14 +3513,14 @@
       </c>
       <c r="F143" s="1">
         <f t="shared" si="23"/>
-        <v>63600</v>
+        <v>15000</v>
       </c>
       <c r="G143" s="1">
         <v>16</v>
       </c>
       <c r="H143" s="16">
         <f t="shared" si="22"/>
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3532,14 +3532,14 @@
       </c>
       <c r="F144" s="1">
         <f t="shared" si="23"/>
-        <v>64400</v>
+        <v>15600</v>
       </c>
       <c r="G144" s="1">
         <v>17</v>
       </c>
       <c r="H144" s="16">
         <f t="shared" si="22"/>
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="145" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3551,14 +3551,14 @@
       </c>
       <c r="F145" s="1">
         <f t="shared" si="23"/>
-        <v>66000</v>
+        <v>16800</v>
       </c>
       <c r="G145" s="1">
         <v>18</v>
       </c>
       <c r="H145" s="16">
         <f t="shared" si="22"/>
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="146" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3570,14 +3570,14 @@
       </c>
       <c r="F146" s="1">
         <f t="shared" si="23"/>
-        <v>66800</v>
+        <v>17400</v>
       </c>
       <c r="G146" s="1">
         <v>18</v>
       </c>
       <c r="H146" s="16">
         <f t="shared" si="22"/>
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="147" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3589,14 +3589,14 @@
       </c>
       <c r="F147" s="1">
         <f t="shared" si="23"/>
-        <v>68400</v>
+        <v>24800</v>
       </c>
       <c r="G147" s="1">
         <v>20</v>
       </c>
       <c r="H147" s="16">
         <f t="shared" si="22"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="148" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3608,14 +3608,14 @@
       </c>
       <c r="F148" s="1">
         <f t="shared" si="23"/>
-        <v>72800</v>
+        <v>29200</v>
       </c>
       <c r="G148" s="1">
         <v>24</v>
       </c>
       <c r="H148" s="16">
         <f t="shared" si="22"/>
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3627,14 +3627,14 @@
       </c>
       <c r="F149" s="1">
         <f t="shared" si="23"/>
-        <v>72800</v>
+        <v>29200</v>
       </c>
       <c r="G149" s="1">
         <v>25</v>
       </c>
       <c r="H149" s="16">
         <f t="shared" si="22"/>
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -3650,7 +3650,7 @@
       </c>
       <c r="E150" s="5">
         <f>($F$2*C150)+($H$2*D150)</f>
-        <v>1290</v>
+        <v>0</v>
       </c>
       <c r="H150" s="16"/>
     </row>
@@ -3663,14 +3663,14 @@
       </c>
       <c r="F151" s="1">
         <f>($E$150+B151)*(IF(B151&lt;=$C$8,1,0)*$D$8+IF(AND(B151&gt;$C$8,B151&lt;=$C$9),1,0)*$D$9+IF(AND(B151&gt;$C$9,B151&lt;=$C$10),1,0)*$D$10+IF(AND(B151&gt;$C$10,B151&lt;=$C$11),1,0)*$D$11+IF(AND(B151&gt;$C$11,B151&lt;=$C$12),1,0)*$D$12+IF(AND(B151&gt;$C$12,B151&lt;=$C$13),1,0)*$D$13+IF(AND(B151&gt;$C$13,B151&lt;=$C$14),1,0)*$D$14+IF(AND(B151&gt;$C$14,B151&lt;=$C$15),1,0)*$D$15+IF(AND(B151&gt;$C$15,B151&lt;=$C$16),1,0)*$D$16+IF(AND(B151&gt;$C$16,B151&lt;=$C$17),1,0)*$D$17)</f>
-        <v>73200</v>
+        <v>16200</v>
       </c>
       <c r="G151" s="1">
         <v>0</v>
       </c>
       <c r="H151" s="16">
         <f>ROUND(((F151-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="152" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3682,14 +3682,14 @@
       </c>
       <c r="F152" s="1">
         <f>($E$150+B152)*(IF(B152&lt;=$C$8,1,0)*$D$8+IF(AND(B152&gt;$C$8,B152&lt;=$C$9),1,0)*$D$9+IF(AND(B152&gt;$C$9,B152&lt;=$C$10),1,0)*$D$10+IF(AND(B152&gt;$C$10,B152&lt;=$C$11),1,0)*$D$11+IF(AND(B152&gt;$C$11,B152&lt;=$C$12),1,0)*$D$12+IF(AND(B152&gt;$C$12,B152&lt;=$C$13),1,0)*$D$13+IF(AND(B152&gt;$C$13,B152&lt;=$C$14),1,0)*$D$14+IF(AND(B152&gt;$C$14,B152&lt;=$C$15),1,0)*$D$15+IF(AND(B152&gt;$C$15,B152&lt;=$C$16),1,0)*$D$16+IF(AND(B152&gt;$C$16,B152&lt;=$C$17),1,0)*$D$17)</f>
-        <v>75600</v>
+        <v>18000</v>
       </c>
       <c r="G152" s="1">
         <v>6</v>
       </c>
       <c r="H152" s="16">
         <f>ROUND(((F152-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3701,14 +3701,14 @@
       </c>
       <c r="F153" s="1">
         <f>($E$150+B153)*(IF(B153&lt;=$C$8,1,0)*$D$8+IF(AND(B153&gt;$C$8,B153&lt;=$C$9),1,0)*$D$9+IF(AND(B153&gt;$C$9,B153&lt;=$C$10),1,0)*$D$10+IF(AND(B153&gt;$C$10,B153&lt;=$C$11),1,0)*$D$11+IF(AND(B153&gt;$C$11,B153&lt;=$C$12),1,0)*$D$12+IF(AND(B153&gt;$C$12,B153&lt;=$C$13),1,0)*$D$13+IF(AND(B153&gt;$C$13,B153&lt;=$C$14),1,0)*$D$14+IF(AND(B153&gt;$C$14,B153&lt;=$C$15),1,0)*$D$15+IF(AND(B153&gt;$C$15,B153&lt;=$C$16),1,0)*$D$16+IF(AND(B153&gt;$C$16,B153&lt;=$C$17),1,0)*$D$17)</f>
-        <v>79600</v>
+        <v>28000</v>
       </c>
       <c r="G153" s="1">
         <v>10</v>
       </c>
       <c r="H153" s="16">
         <f>ROUND(((F153-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="154" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3720,7 +3720,7 @@
       </c>
       <c r="F154" s="1">
         <f>($E$150+B154)*(IF(B154&lt;=$C$8,1,0)*$D$8+IF(AND(B154&gt;$C$8,B154&lt;=$C$9),1,0)*$D$9+IF(AND(B154&gt;$C$9,B154&lt;=$C$10),1,0)*$D$10+IF(AND(B154&gt;$C$10,B154&lt;=$C$11),1,0)*$D$11+IF(AND(B154&gt;$C$11,B154&lt;=$C$12),1,0)*$D$12+IF(AND(B154&gt;$C$12,B154&lt;=$C$13),1,0)*$D$13+IF(AND(B154&gt;$C$13,B154&lt;=$C$14),1,0)*$D$14+IF(AND(B154&gt;$C$14,B154&lt;=$C$15),1,0)*$D$15+IF(AND(B154&gt;$C$15,B154&lt;=$C$16),1,0)*$D$16+IF(AND(B154&gt;$C$16,B154&lt;=$C$17),1,0)*$D$17)</f>
-        <v>81600</v>
+        <v>30000</v>
       </c>
       <c r="G154" s="1">
         <v>16</v>
@@ -3743,7 +3743,7 @@
       </c>
       <c r="E155" s="5">
         <f>($F$2*C155)+($H$2*D155)</f>
-        <v>1170</v>
+        <v>0</v>
       </c>
       <c r="H155" s="16"/>
     </row>
@@ -3756,14 +3756,14 @@
       </c>
       <c r="F156" s="1">
         <f>($E$155+B156)*(IF(B156&lt;=$C$8,1,0)*$D$8+IF(AND(B156&gt;$C$8,B156&lt;=$C$9),1,0)*$D$9+IF(AND(B156&gt;$C$9,B156&lt;=$C$10),1,0)*$D$10+IF(AND(B156&gt;$C$10,B156&lt;=$C$11),1,0)*$D$11+IF(AND(B156&gt;$C$11,B156&lt;=$C$12),1,0)*$D$12+IF(AND(B156&gt;$C$12,B156&lt;=$C$13),1,0)*$D$13+IF(AND(B156&gt;$C$13,B156&lt;=$C$14),1,0)*$D$14+IF(AND(B156&gt;$C$14,B156&lt;=$C$15),1,0)*$D$15+IF(AND(B156&gt;$C$15,B156&lt;=$C$16),1,0)*$D$16+IF(AND(B156&gt;$C$16,B156&lt;=$C$17),1,0)*$D$17)</f>
-        <v>25440</v>
+        <v>4200</v>
       </c>
       <c r="G156" s="1">
         <v>0</v>
       </c>
       <c r="H156" s="16">
         <f t="shared" ref="H156:H164" si="24">ROUND(((F156-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3775,14 +3775,14 @@
       </c>
       <c r="F157" s="1">
         <f t="shared" ref="F157:F164" si="25">($E$155+B157)*(IF(B157&lt;=$C$8,1,0)*$D$8+IF(AND(B157&gt;$C$8,B157&lt;=$C$9),1,0)*$D$9+IF(AND(B157&gt;$C$9,B157&lt;=$C$10),1,0)*$D$10+IF(AND(B157&gt;$C$10,B157&lt;=$C$11),1,0)*$D$11+IF(AND(B157&gt;$C$11,B157&lt;=$C$12),1,0)*$D$12+IF(AND(B157&gt;$C$12,B157&lt;=$C$13),1,0)*$D$13+IF(AND(B157&gt;$C$13,B157&lt;=$C$14),1,0)*$D$14+IF(AND(B157&gt;$C$14,B157&lt;=$C$15),1,0)*$D$15+IF(AND(B157&gt;$C$15,B157&lt;=$C$16),1,0)*$D$16+IF(AND(B157&gt;$C$16,B157&lt;=$C$17),1,0)*$D$17)</f>
-        <v>65200</v>
+        <v>9200</v>
       </c>
       <c r="G157" s="1">
         <v>0</v>
       </c>
       <c r="H157" s="16">
         <f t="shared" si="24"/>
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="158" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3794,14 +3794,14 @@
       </c>
       <c r="F158" s="1">
         <f t="shared" si="25"/>
-        <v>65200</v>
+        <v>9200</v>
       </c>
       <c r="G158" s="1">
         <v>2</v>
       </c>
       <c r="H158" s="16">
         <f t="shared" si="24"/>
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="159" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3813,14 +3813,14 @@
       </c>
       <c r="F159" s="1">
         <f t="shared" si="25"/>
-        <v>66800</v>
+        <v>15000</v>
       </c>
       <c r="G159" s="1">
         <v>6</v>
       </c>
       <c r="H159" s="16">
         <f t="shared" si="24"/>
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="160" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3832,14 +3832,14 @@
       </c>
       <c r="F160" s="1">
         <f t="shared" si="25"/>
-        <v>68400</v>
+        <v>16200</v>
       </c>
       <c r="G160" s="1">
         <v>6</v>
       </c>
       <c r="H160" s="16">
         <f t="shared" si="24"/>
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3851,14 +3851,14 @@
       </c>
       <c r="F161" s="1">
         <f t="shared" si="25"/>
-        <v>68400</v>
+        <v>16200</v>
       </c>
       <c r="G161" s="1">
         <v>11</v>
       </c>
       <c r="H161" s="16">
         <f t="shared" si="24"/>
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3870,14 +3870,14 @@
       </c>
       <c r="F162" s="1">
         <f t="shared" si="25"/>
-        <v>70800</v>
+        <v>18000</v>
       </c>
       <c r="G162" s="1">
         <v>10</v>
       </c>
       <c r="H162" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="163" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3889,14 +3889,14 @@
       </c>
       <c r="F163" s="1">
         <f t="shared" si="25"/>
-        <v>74800</v>
+        <v>28000</v>
       </c>
       <c r="G163" s="1">
         <v>16</v>
       </c>
       <c r="H163" s="16">
         <f t="shared" si="24"/>
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="164" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3908,14 +3908,14 @@
       </c>
       <c r="F164" s="1">
         <f t="shared" si="25"/>
-        <v>76800</v>
+        <v>30000</v>
       </c>
       <c r="G164" s="1">
         <v>16</v>
       </c>
       <c r="H164" s="16">
         <f t="shared" si="24"/>
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>